<commit_message>
up: phase et activité
</commit_message>
<xml_diff>
--- a/data/doc for notification1.xlsx
+++ b/data/doc for notification1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Tsikilo\Tsikilo code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Tsikilo\Tsikilo code\tsikilo-front\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36387A64-35C5-4B0F-85E1-02AA88037AFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E7A369-C14D-49F1-AF8F-57B22250694B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7425" yWindow="0" windowWidth="21480" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -437,6 +437,37 @@
   </si>
   <si>
     <t>La phase '[Nom de la phase]' du projet '[Nom du projet]' est terminée. ✅ Cliquez ici pour consulter les détails</t>
+  </si>
+  <si>
+    <t>Votre tâche '[Nom de la tâche]' a été créée avec succès. 📋 Cliquez ici pour consulter ou modifier les détails</t>
+  </si>
+  <si>
+    <t>Une nouvelle tâche '[Nom de la tâche]' vous a été assignée dans le projet '[Nom du projet]'. 📋 Cliquez ici pour consulter les détails.</t>
+  </si>
+  <si>
+    <t>Objet : Une nouvelle tâche vous a été assignée dans le projet '[Nom du projet]'
+Bonjour [Prénom Nom],
+Une nouvelle tâche vous a été assignée dans le projet [Nom du projet].
+Détails de la tâche :
+•	Nom de la tâche : [Nom de la tâche]
+•	Assignée par : [Votre Prénom et Nom]
+•	Date d'échéance : [Date d'échéance ou "Aucune échéance précisée"]
+•	Priorité : [Priorité, par exemple : Haute, Moyenne, Basse]
+•	Description : [Courte description ou objectifs de la tâche, si applicables]
+Vous pouvez consulter les détails de la tâche et suivre son avancement ici :
+Accéder à la tâche</t>
+  </si>
+  <si>
+    <t>La tâche '[Nom de la tâche]' associée à vous dans le projet '[Nom du projet]' a été modifiée. ✏️ Cliquez ici pour consulter les mises à jour</t>
+  </si>
+  <si>
+    <t>Une activité transverse/intercontrat de type [type] vous a été assigné. Cliquez ici pour consulter les détails</t>
+  </si>
+  <si>
+    <t>Une activité transverse/intercontrat associé a vous :[titre] a été modifiée. Cliquez ici pour consulter les mises à jour.</t>
+  </si>
+  <si>
+    <t>Une activité transverse/intercontrat associé a vous :[titre] a été supprimée. Cliquez ici pour consulter les mises à jour.</t>
   </si>
 </sst>
 </file>
@@ -582,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -592,15 +623,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -618,6 +640,18 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -906,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -944,260 +978,260 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
     </row>
     <row r="3" spans="1:7" ht="195">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="165">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="D4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="8" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="210">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="5" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="13" t="s">
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="5" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="240">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="12" t="s">
+      <c r="F9" s="9" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="210">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="D10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="8" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="195">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="D11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="G11" s="8" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="270">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="D12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="5" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="255">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="12" t="s">
+      <c r="D13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="G13" s="8" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1217,144 +1251,165 @@
       <c r="E14" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="5" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+    </row>
+    <row r="16" spans="1:7" ht="45">
+      <c r="A16" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="1" t="s">
+      <c r="D16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" t="s">
+      <c r="F16" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="240">
+      <c r="A17" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" t="s">
+      <c r="D17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="60">
+      <c r="A18" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="D18" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="F18" s="9" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="18.75">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="6"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:7" ht="45">
+      <c r="A20" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E20" s="1" t="s">
+      <c r="D20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" t="s">
+      <c r="F20" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45">
+      <c r="A21" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D21" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="1" t="s">
+      <c r="D21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" t="s">
+      <c r="F21" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="45">
+      <c r="A22" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="1" t="s">
+      <c r="D22" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>21</v>
       </c>
+      <c r="F22" s="9" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="18.75">
-      <c r="A25" s="7" t="s">
+      <c r="A25" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" t="s">

</xml_diff>

<commit_message>
up: doc notification update content
</commit_message>
<xml_diff>
--- a/data/doc for notification1.xlsx
+++ b/data/doc for notification1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Tsikilo\Tsikilo code\tsikilo-front\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E7A369-C14D-49F1-AF8F-57B22250694B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201B25F0-FB6C-4ABF-9EEF-BD4FFF07E380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7425" yWindow="0" windowWidth="21480" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="87">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>O/jour</t>
-  </si>
-  <si>
-    <t>Quand une phase vient d'être terminé</t>
   </si>
   <si>
     <t>Débloquer un projet</t>
@@ -377,48 +374,10 @@
     <t>Félicitations ! Le projet '[Nom du projet]' est maintenant terminé. 🎉 Cliquez ici pour voir les détails.</t>
   </si>
   <si>
-    <t>Objet : Félicitations ! Le projet '[Nom du projet]' est terminé
-Bonjour [Prénom Nom],
-Nous sommes heureux de vous annoncer que le projet [Nom du projet] a atteint 100% d'avancement et est désormais terminé. 🎉
-Détails :
-•	Date de fin : [Date de fin du projet]
-•	État du projet : Terminé (100% d'avancement)
-•	Résumé des réalisations :
-o	[Bref résumé des résultats du projet, si souhaité]
-o	[Remerciements ou points marquants si pertinent]
-Vous pouvez consulter le projet pour voir les dernières mises à jour et les résultats finaux :
-Accéder au projet</t>
-  </si>
-  <si>
     <t>Le projet '[Nom du projet]' a été archivé. 🗃️ Cliquez ici pour consulter les détails.</t>
   </si>
   <si>
-    <t>Objet : Le projet '[Nom du projet]' a été archivé
-Bonjour [Prénom Nom],
-Nous vous informons que le projet [Nom du projet] a été archivé. Il n'est plus actif, mais vous pouvez toujours consulter ses détails à tout moment. 🗃️
-Détails :
-•	Date de l'archivage : [Date d'archivage]
-•	État du projet : Archivé
-•	Résumé du projet :
-o	[Bref résumé des résultats du projet, s'il y en a]
-o	[Éventuellement des actions recommandées ou à venir]
-Vous pouvez consulter les détails du projet archivé ici :
-Accéder au projet archivé</t>
-  </si>
-  <si>
     <t>Le projet '[Nom du projet]' est désormais en stand-by. ⏸️ Cliquez ici pour consulter les détails.</t>
-  </si>
-  <si>
-    <t>Objet : Le projet '[Nom du projet]' est mis en stand-by
-Bonjour [Prénom Nom],
-Nous vous informons que le projet [Nom du projet] est actuellement mis en stand-by pour une durée indéterminée.
-Détails :
-Date de mise en stand-by : [Date de mise en stand-by]
-État du projet : En stand-by
-Raison de la mise en stand-by : [Optionnel : explication succincte, par exemple : "En attente de ressources", "Révision stratégique", etc.]
-Période estimée de reprise : [Optionnel : si vous avez une estimation, sinon indiquez que la durée est indéterminée]
-Vous pouvez toujours consulter les détails du projet pendant cette période :
-Accéder au projet en stand-by</t>
   </si>
   <si>
     <t>Le projet '[Nom du projet]' a été débloqué et est de nouveau actif. 🚀 Cliquez ici pour consulter les détails.</t>
@@ -434,9 +393,6 @@
 •	Prochaines étapes : [Optionnel : informations supplémentaires sur les étapes suivantes ou un plan d'action]
 Vous pouvez consulter les détails du projet maintenant qu'il est à nouveau actif :
 Accéder au projet débloqué</t>
-  </si>
-  <si>
-    <t>La phase '[Nom de la phase]' du projet '[Nom du projet]' est terminée. ✅ Cliquez ici pour consulter les détails</t>
   </si>
   <si>
     <t>Votre tâche '[Nom de la tâche]' a été créée avec succès. 📋 Cliquez ici pour consulter ou modifier les détails</t>
@@ -468,6 +424,52 @@
   </si>
   <si>
     <t>Une activité transverse/intercontrat associé a vous :[titre] a été supprimée. Cliquez ici pour consulter les mises à jour.</t>
+  </si>
+  <si>
+    <t>Le projet '[Nom du projet]' arrive a échéance.  Cliquez ici pour consulter les détails.</t>
+  </si>
+  <si>
+    <t>Le projet '[Nom du projet]' connais un retard de [nbrDeJour] jours. 🚀 Cliquez ici pour consulter les détails.</t>
+  </si>
+  <si>
+    <t>La phase '[Nom de la phase]' du projet '[Nom du projet]' est [status De la phase]. ✅ Cliquez ici pour consulter les détails</t>
+  </si>
+  <si>
+    <t>La tâche '[Nom de la tâche]' associée à vous dans le projet '[Nom du projet]' approche de sa date d'échéance. ✏️ Cliquez ici pour consulter les mises à jour</t>
+  </si>
+  <si>
+    <t>La tâche '[Nom de la tâche]' associée à vous dans le projet '[Nom du projet]' est en retard de [nbr de jour] jours. ✏️ Cliquez ici pour consulter les mises à jour</t>
+  </si>
+  <si>
+    <t>Objet : Félicitations ! Le projet '[Nom du projet]' est terminé
+Bonjour [Prénom Nom],
+Nous sommes heureux de vous annoncer que le projet [Nom du projet] a atteint 100% d'avancement et est désormais terminé. 🎉
+Détails :
+•	Date de fin : [Date de fin du projet]
+•	État du projet : Terminé (100% d'avancement)
+Vous pouvez consulter le projet pour voir les dernières mises à jour et les résultats finaux :
+Accéder au projet</t>
+  </si>
+  <si>
+    <t>Objet : Le projet '[Nom du projet]' a été archivé
+Bonjour [Prénom Nom],
+Nous vous informons que le projet [Nom du projet] a été archivé. Il n'est plus actif, mais vous pouvez toujours consulter ses détails à tout moment. 🗃️
+Détails :
+•	Date de l'archivage : [Date d'archivage]
+•	État du projet : Archivé
+Vous pouvez consulter les détails du projet archivé ici :
+Accéder au projet archivé</t>
+  </si>
+  <si>
+    <t>Objet : Le projet '[Nom du projet]' est mis en stand-by
+Bonjour [Prénom Nom],
+Nous vous informons que le projet [Nom du projet] est actuellement mis en stand-by pour une durée indéterminée.
+Détails :
+Date de mise en stand-by : [Date de mise en stand-by]
+État du projet : En stand-by
+Raison de la mise en stand-by : [Optionnel : explication succincte, par exemple : "En attente de ressources", "Révision stratégique", etc.]
+Vous pouvez toujours consulter les détails du projet pendant cette période :
+Accéder au projet en stand-by</t>
   </si>
 </sst>
 </file>
@@ -613,7 +615,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -649,9 +651,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,10 +937,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="D12" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1005,10 +1004,10 @@
         <v>11</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="165">
@@ -1028,10 +1027,10 @@
         <v>11</v>
       </c>
       <c r="F4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="210">
@@ -1051,10 +1050,10 @@
         <v>11</v>
       </c>
       <c r="F5" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>60</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5">
@@ -1074,10 +1073,10 @@
         <v>11</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="240">
@@ -1097,10 +1096,10 @@
         <v>11</v>
       </c>
       <c r="F7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="30">
@@ -1120,7 +1119,7 @@
         <v>21</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="45">
@@ -1140,10 +1139,10 @@
         <v>21</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="210">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="165">
       <c r="A10" s="7" t="s">
         <v>22</v>
       </c>
@@ -1160,13 +1159,13 @@
         <v>11</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="195">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="150">
       <c r="A11" s="7" t="s">
         <v>26</v>
       </c>
@@ -1183,13 +1182,13 @@
         <v>11</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="270">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="255">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -1206,18 +1205,18 @@
         <v>11</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="255">
       <c r="A13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>52</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>53</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>25</v>
@@ -1229,30 +1228,30 @@
         <v>11</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="45">
-      <c r="A14" t="s">
+      <c r="A14" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="1" t="s">
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>76</v>
+      <c r="F14" s="9" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
@@ -1283,7 +1282,7 @@
         <v>21</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="240">
@@ -1303,10 +1302,10 @@
         <v>11</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="60">
@@ -1326,7 +1325,7 @@
         <v>21</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18.75">
@@ -1356,8 +1355,8 @@
       <c r="E20" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F20" s="14" t="s">
-        <v>81</v>
+      <c r="F20" s="9" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="45">
@@ -1377,7 +1376,7 @@
         <v>21</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="45">
@@ -1397,7 +1396,7 @@
         <v>21</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18.75">
@@ -1411,74 +1410,73 @@
       <c r="F25" s="13"/>
       <c r="G25" s="13"/>
     </row>
-    <row r="26" spans="1:7">
-      <c r="B26" t="s">
+    <row r="26" spans="1:7" ht="30">
+      <c r="A26" s="7"/>
+      <c r="B26" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="1" t="s">
+      <c r="D26" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="B27" t="s">
+      <c r="F26" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="45">
+      <c r="B27" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="D27" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="B28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="E27" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="60">
+      <c r="B28" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="1" t="s">
+      <c r="D28" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="B29" t="s">
+      <c r="F28" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60">
+      <c r="B29" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C29" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="1" t="s">
+      <c r="C29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E29" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="B30" t="s">
-        <v>55</v>
-      </c>
-      <c r="C30" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>21</v>
+      <c r="F29" s="9" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update(doc notification): archive and project state
</commit_message>
<xml_diff>
--- a/data/doc for notification1.xlsx
+++ b/data/doc for notification1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Tsikilo\Tsikilo code\tsikilo-front\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C86548-1B72-4F4D-A56C-807CD99B954F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7970B5-C3E0-41F7-BBB5-55AF2769B336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="101">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -467,9 +467,6 @@
 Accéder au projet débloqué</t>
   </si>
   <si>
-    <t>Toute personne dans le projet(N+1 et N+2)</t>
-  </si>
-  <si>
     <t>Chef de projet (N+1 et N+2)</t>
   </si>
   <si>
@@ -501,13 +498,73 @@
   </si>
   <si>
     <t>T  A  C  H  E</t>
+  </si>
+  <si>
+    <r>
+      <t>Chef de projet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (N+1 et N+2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Toute personne dans le projet</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(N+1 et N+2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Toute l'équipe du projet  </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(N+1 et N+2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Toute l'équipe du projet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (N+1 et N+2)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,8 +630,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +672,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -652,7 +722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -676,9 +746,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -705,6 +772,15 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -713,6 +789,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF0000"/>
       <color rgb="FF4EA72E"/>
     </mruColors>
   </colors>
@@ -992,8 +1069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1030,33 +1107,33 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
     <row r="3" spans="1:7" ht="195">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="9" t="s">
+      <c r="C3" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>55</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -1064,68 +1141,68 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="165">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="D4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="210">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="D5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="D6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="21" t="s">
         <v>61</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -1133,25 +1210,25 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="240">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="D7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="G7" s="12" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1176,43 +1253,43 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="45">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="9" t="s">
+      <c r="C9" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="15"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" ht="165">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="C10" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="20" t="s">
         <v>66</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1220,22 +1297,22 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="150">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="C11" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="20" t="s">
         <v>67</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -1250,7 +1327,7 @@
         <v>28</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>11</v>
@@ -1273,7 +1350,7 @@
         <v>51</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>11</v>
@@ -1296,7 +1373,7 @@
         <v>30</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>11</v>
@@ -1309,15 +1386,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
     </row>
     <row r="16" spans="1:7" ht="45">
       <c r="A16" s="6" t="s">
@@ -1364,10 +1441,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>32</v>
@@ -1383,7 +1460,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>45</v>
@@ -1426,15 +1503,15 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
     </row>
     <row r="23" spans="1:7" ht="45">
       <c r="A23" s="7" t="s">
@@ -1497,15 +1574,15 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
     </row>
     <row r="29" spans="1:7" ht="30">
       <c r="A29" s="7"/>
@@ -1530,7 +1607,7 @@
         <v>47</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>49</v>
@@ -1541,7 +1618,7 @@
       <c r="F30" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="G30" s="15"/>
+      <c r="G30" s="14"/>
     </row>
     <row r="31" spans="1:7" ht="60">
       <c r="B31" s="7" t="s">
@@ -1565,7 +1642,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>49</v>
@@ -1576,22 +1653,22 @@
       <c r="F32" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="15"/>
+      <c r="G32" s="14"/>
     </row>
     <row r="35" spans="1:7" ht="18.75">
-      <c r="A35" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="B35" s="19"/>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
+      <c r="A35" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="18"/>
+      <c r="C35" s="18"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>14</v>
@@ -1600,12 +1677,12 @@
         <v>21</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
up(notificationMessage): notif when status phase change
</commit_message>
<xml_diff>
--- a/data/doc for notification1.xlsx
+++ b/data/doc for notification1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Tsikilo\Tsikilo code\tsikilo-front\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7970B5-C3E0-41F7-BBB5-55AF2769B336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7A5807A-5CD6-44CD-9336-C95BB463EAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="100">
   <si>
     <t>Fonctionnalité</t>
   </si>
@@ -467,12 +467,6 @@
 Accéder au projet débloqué</t>
   </si>
   <si>
-    <t>Chef de projet (N+1 et N+2)</t>
-  </si>
-  <si>
-    <t>Toute l'équipe du projet  (N+1 et N+2)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Toute personne dans le projet  </t>
   </si>
   <si>
@@ -557,6 +551,21 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> (N+1 et N+2)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Chef de projet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(N+1 et N+2)</t>
     </r>
   </si>
 </sst>
@@ -763,6 +772,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -772,15 +790,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,8 +798,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4EA72E"/>
       <color rgb="FFFF0000"/>
-      <color rgb="FF4EA72E"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1069,8 +1078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1107,33 +1116,33 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" ht="195">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="20" t="s">
+      <c r="C3" s="16" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>55</v>
       </c>
       <c r="G3" s="9" t="s">
@@ -1187,22 +1196,22 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="409.5">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="19" t="s">
+      <c r="C6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="21" t="s">
+      <c r="D6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="18" t="s">
         <v>61</v>
       </c>
       <c r="G6" s="5" t="s">
@@ -1253,43 +1262,43 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="45">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="14"/>
+    </row>
+    <row r="10" spans="1:7" ht="165">
+      <c r="A10" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="165">
-      <c r="A10" s="19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" s="20" t="s">
+      <c r="D10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>66</v>
       </c>
       <c r="G10" s="8" t="s">
@@ -1297,22 +1306,22 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="150">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="20" t="s">
+      <c r="C11" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>67</v>
       </c>
       <c r="G11" s="8" t="s">
@@ -1320,22 +1329,22 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="255">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="C12" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>68</v>
       </c>
       <c r="G12" s="5" t="s">
@@ -1343,22 +1352,22 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="210">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F13" s="9" t="s">
+      <c r="C13" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>69</v>
       </c>
       <c r="G13" s="8" t="s">
@@ -1366,35 +1375,35 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="45">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="C14" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="F14" s="17" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="18.75">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
     </row>
     <row r="16" spans="1:7" ht="45">
       <c r="A16" s="6" t="s">
@@ -1441,10 +1450,10 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>32</v>
@@ -1460,7 +1469,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>45</v>
@@ -1503,15 +1512,15 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="18.75">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="17"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
     </row>
     <row r="23" spans="1:7" ht="45">
       <c r="A23" s="7" t="s">
@@ -1574,15 +1583,15 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="18.75">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
-      <c r="D28" s="18"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="18"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
     </row>
     <row r="29" spans="1:7" ht="30">
       <c r="A29" s="7"/>
@@ -1607,7 +1616,7 @@
         <v>47</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>49</v>
@@ -1642,7 +1651,7 @@
         <v>53</v>
       </c>
       <c r="C32" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>49</v>
@@ -1656,19 +1665,19 @@
       <c r="G32" s="14"/>
     </row>
     <row r="35" spans="1:7" ht="18.75">
-      <c r="A35" s="18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="A35" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
     </row>
     <row r="36" spans="1:7">
       <c r="B36" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>14</v>
@@ -1677,12 +1686,12 @@
         <v>21</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="B37" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
up(docnotif): mail create project
</commit_message>
<xml_diff>
--- a/data/doc for notification1.xlsx
+++ b/data/doc for notification1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projet\Tsikilo\Tsikilo code\tsikilo-front\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394218F4-2BC9-4941-B3AA-4780E8CB72AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E64ACE5-51F1-40B7-AE9E-FA25C2D68D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -148,18 +148,6 @@
   </si>
   <si>
     <t>Quand une phase est en retard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Objet : Projet sur GMP : {titre projet}
-Bonjour, {nom}
-Nous avons le plaisir de vous informer que votre projet intitulé [Nom du projet] a été créé avec succès.
-Détails du projet :
-•	Nom du projet : [Nom du projet]
-•	Description : [Description du projet]
-•	Date de création : [Date]
-•	Responsable : [Nom du responsable]
-Vous pouvez dès à présent accéder à votre projet via l’application de gestion et management de projet (G.M.P)
-</t>
   </si>
   <si>
     <t>•	CDP : Votre projet '[Nom du projet]' a été créé avec succès ! 🎉 Vous êtes le responsable de ce projet. Cliquez ici pour le gérer.
@@ -561,6 +549,18 @@
   </si>
   <si>
     <t>Toute personne dans le projet - observateur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Objet : Projet sur GMP : {titre projet}
+Bonjour, {nom}
+Nous avons le plaisir de vous informer que votre projet intitulé [Nom du projet] a été créé avec succès.
+Détails du projet :
+•	Nom du projet : [Nom du projet]
+•	Description : [Description du projet]
+•	Date de création : [Date]
+•	Responsable : [Nom du responsable]
+Vous pouvez dès à présent accéder à votre projet via l’application de gestion et management de projet (G.M.P)     CTA
+</t>
   </si>
 </sst>
 </file>
@@ -719,7 +719,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -766,20 +766,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,8 +1063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1091,10 +1085,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>2</v>
@@ -1110,18 +1104,18 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-    </row>
-    <row r="3" spans="1:8" ht="195">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+    </row>
+    <row r="3" spans="1:8" ht="210">
       <c r="A3" s="12" t="s">
         <v>7</v>
       </c>
@@ -1129,10 +1123,10 @@
         <v>8</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>9</v>
@@ -1141,10 +1135,10 @@
         <v>9</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H3" s="9" t="s">
         <v>41</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="165">
@@ -1155,10 +1149,10 @@
         <v>11</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>9</v>
@@ -1167,10 +1161,10 @@
         <v>9</v>
       </c>
       <c r="G4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="210">
@@ -1181,10 +1175,10 @@
         <v>13</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>9</v>
@@ -1193,10 +1187,10 @@
         <v>9</v>
       </c>
       <c r="G5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="409.5">
@@ -1207,10 +1201,10 @@
         <v>14</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>9</v>
@@ -1219,10 +1213,10 @@
         <v>9</v>
       </c>
       <c r="G6" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="240">
@@ -1233,10 +1227,10 @@
         <v>15</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>9</v>
@@ -1245,10 +1239,10 @@
         <v>9</v>
       </c>
       <c r="G7" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30">
@@ -1269,7 +1263,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="45">
@@ -1280,7 +1274,7 @@
         <v>20</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12" t="s">
@@ -1290,7 +1284,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H9" s="11"/>
     </row>
@@ -1302,7 +1296,7 @@
         <v>21</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D10" s="12"/>
       <c r="E10" s="12" t="s">
@@ -1312,10 +1306,10 @@
         <v>9</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="150">
@@ -1326,7 +1320,7 @@
         <v>23</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D11" s="12"/>
       <c r="E11" s="12" t="s">
@@ -1336,10 +1330,10 @@
         <v>9</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="255">
@@ -1350,7 +1344,7 @@
         <v>25</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12" t="s">
@@ -1360,10 +1354,10 @@
         <v>9</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="210">
@@ -1374,7 +1368,7 @@
         <v>38</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="12"/>
       <c r="E13" s="12" t="s">
@@ -1384,10 +1378,10 @@
         <v>9</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="45">
@@ -1398,7 +1392,7 @@
         <v>27</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12" t="s">
@@ -1408,20 +1402,20 @@
         <v>18</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="18.75">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8" ht="240">
       <c r="A16" s="12" t="s">
@@ -1441,18 +1435,18 @@
         <v>9</v>
       </c>
       <c r="G16" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="30">
       <c r="A17" s="16" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>29</v>
@@ -1469,7 +1463,7 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>33</v>
@@ -1489,7 +1483,7 @@
     </row>
     <row r="19" spans="1:8" ht="60">
       <c r="A19" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>30</v>
@@ -1505,20 +1499,20 @@
         <v>18</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="18.75">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
+      <c r="B20" s="18"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
     </row>
     <row r="21" spans="1:8" ht="30">
       <c r="A21" s="7"/>
@@ -1526,7 +1520,7 @@
         <v>36</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>12</v>
@@ -1538,7 +1532,7 @@
         <v>18</v>
       </c>
       <c r="G21" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="45">
@@ -1546,19 +1540,19 @@
         <v>35</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D22" s="17" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>86</v>
+        <v>94</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="G22" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="60">
@@ -1566,7 +1560,7 @@
         <v>39</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="12" t="s">
@@ -1576,7 +1570,7 @@
         <v>18</v>
       </c>
       <c r="G23" s="13" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="60">
@@ -1584,64 +1578,64 @@
         <v>40</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D24" s="17"/>
       <c r="E24" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="F24" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="F24" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H24" s="11"/>
     </row>
     <row r="27" spans="1:8" ht="18.75">
-      <c r="A27" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="21"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="21"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
+      <c r="A27" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8" ht="30">
       <c r="B28" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F28" s="16" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="45">
       <c r="B29" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>93</v>
-      </c>
       <c r="D29" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>18</v>
       </c>
       <c r="F29" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>